<commit_message>
moved 108 from kvlinden to fsantos
</commit_message>
<xml_diff>
--- a/data/schedule_2025.xlsx
+++ b/data/schedule_2025.xlsx
@@ -1679,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" xml:space="preserve">
       <c r="A19" t="str">
         <v>Computer Science</v>
       </c>
@@ -1713,8 +1713,10 @@
       <c r="K19" t="str">
         <v/>
       </c>
-      <c r="L19" t="str">
-        <v>MTWRF</v>
+      <c r="L19" t="str" xml:space="preserve">
+        <v xml:space="preserve">MTWRF
+MWF
+TR</v>
       </c>
       <c r="M19" t="str">
         <v>16:00:00</v>
@@ -1723,7 +1725,7 @@
         <v>135</v>
       </c>
       <c r="O19" t="str">
-        <v>, ,</v>
+        <v xml:space="preserve">, , </v>
       </c>
       <c r="P19" t="str">
         <v/>
@@ -1750,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" xml:space="preserve">
       <c r="A20" t="str">
         <v>Computer Science</v>
       </c>
@@ -1784,8 +1786,10 @@
       <c r="K20" t="str">
         <v/>
       </c>
-      <c r="L20" t="str">
-        <v>MTWRF</v>
+      <c r="L20" t="str" xml:space="preserve">
+        <v xml:space="preserve">MTWRF
+MWF
+TR</v>
       </c>
       <c r="M20" t="str">
         <v>16:00:00</v>
@@ -1794,7 +1798,7 @@
         <v>135</v>
       </c>
       <c r="O20" t="str">
-        <v>, ,</v>
+        <v xml:space="preserve">, , </v>
       </c>
       <c r="P20" t="str">
         <v/>
@@ -2696,7 +2700,7 @@
         <v>B</v>
       </c>
       <c r="H33" t="str">
-        <v>Keith VanderLinden</v>
+        <v>Fernando Pasquini Santos</v>
       </c>
       <c r="I33" t="str">
         <v>4</v>
@@ -3880,7 +3884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" xml:space="preserve">
       <c r="A50" t="str">
         <v>Computer Science</v>
       </c>
@@ -3914,8 +3918,9 @@
       <c r="K50" t="str">
         <v/>
       </c>
-      <c r="L50" t="str">
-        <v>MW</v>
+      <c r="L50" t="str" xml:space="preserve">
+        <v xml:space="preserve">MW
+F</v>
       </c>
       <c r="M50" t="str">
         <v>14:45:00</v>
@@ -3951,7 +3956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" xml:space="preserve">
       <c r="A51" t="str">
         <v>Computer Science</v>
       </c>
@@ -3985,8 +3990,9 @@
       <c r="K51" t="str">
         <v/>
       </c>
-      <c r="L51" t="str">
-        <v>F</v>
+      <c r="L51" t="str" xml:space="preserve">
+        <v xml:space="preserve">F
+MW</v>
       </c>
       <c r="M51" t="str">
         <v>14:45:00</v>
@@ -4066,7 +4072,7 @@
         <v>65</v>
       </c>
       <c r="O52" t="str">
-        <v>SB 372</v>
+        <v>NH 64</v>
       </c>
       <c r="P52" t="str">
         <v>Operating Systems and Networki</v>
@@ -4164,7 +4170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" xml:space="preserve">
       <c r="A54" t="str">
         <v>Computer Science</v>
       </c>
@@ -4198,8 +4204,9 @@
       <c r="K54" t="str">
         <v/>
       </c>
-      <c r="L54" t="str">
-        <v>F</v>
+      <c r="L54" t="str" xml:space="preserve">
+        <v xml:space="preserve">F
+MW</v>
       </c>
       <c r="M54" t="str">
         <v>13:30:00</v>
@@ -4235,7 +4242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" xml:space="preserve">
       <c r="A55" t="str">
         <v>Computer Science</v>
       </c>
@@ -4269,8 +4276,9 @@
       <c r="K55" t="str">
         <v/>
       </c>
-      <c r="L55" t="str">
-        <v>MW</v>
+      <c r="L55" t="str" xml:space="preserve">
+        <v xml:space="preserve">MW
+F</v>
       </c>
       <c r="M55" t="str">
         <v>14:45:00</v>
@@ -4912,13 +4920,13 @@
         <v>MWF</v>
       </c>
       <c r="M64" t="str">
-        <v>09:15:00</v>
+        <v>13:30:00</v>
       </c>
       <c r="N64">
         <v>65</v>
       </c>
       <c r="O64" t="str">
-        <v>SB 382</v>
+        <v>SB 372</v>
       </c>
       <c r="P64" t="str">
         <v>Database Management Systems</v>
@@ -4953,46 +4961,46 @@
         <v/>
       </c>
       <c r="C65" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D65" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="E65" t="str">
         <v>CS</v>
       </c>
       <c r="F65" t="str">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="G65" t="str">
         <v>A</v>
       </c>
       <c r="H65" t="str">
-        <v>Harry Plantinga</v>
+        <v>Brian D Paige, Adam Vedra</v>
       </c>
       <c r="I65" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J65" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K65" t="str">
         <v/>
       </c>
       <c r="L65" t="str">
-        <v>MWF</v>
+        <v>MR</v>
       </c>
       <c r="M65" t="str">
-        <v>09:15:00</v>
+        <v>19:00:00</v>
       </c>
       <c r="N65">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O65" t="str">
-        <v>SB 382</v>
+        <v>SB 372</v>
       </c>
       <c r="P65" t="str">
-        <v>Computer Graphics</v>
+        <v>Computer Security</v>
       </c>
       <c r="Q65" t="str">
         <v/>
@@ -5024,22 +5032,22 @@
         <v/>
       </c>
       <c r="C66" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D66" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E66" t="str">
         <v>CS</v>
       </c>
       <c r="F66" t="str">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G66" t="str">
         <v>A</v>
       </c>
       <c r="H66" t="str">
-        <v>Joel Adams</v>
+        <v>Harry Plantinga</v>
       </c>
       <c r="I66" t="str">
         <v>2</v>
@@ -5054,7 +5062,7 @@
         <v>MWF</v>
       </c>
       <c r="M66" t="str">
-        <v>14:45:00</v>
+        <v>09:15:00</v>
       </c>
       <c r="N66">
         <v>65</v>
@@ -5063,7 +5071,7 @@
         <v>SB 382</v>
       </c>
       <c r="P66" t="str">
-        <v>High Performance Computing</v>
+        <v>Computer Graphics</v>
       </c>
       <c r="Q66" t="str">
         <v/>
@@ -5095,22 +5103,22 @@
         <v/>
       </c>
       <c r="C67" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D67" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="E67" t="str">
         <v>CS</v>
       </c>
       <c r="F67" t="str">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G67" t="str">
         <v>A</v>
       </c>
       <c r="H67" t="str">
-        <v>Kenneth C Arnold</v>
+        <v>Joel Adams</v>
       </c>
       <c r="I67" t="str">
         <v>2</v>
@@ -5125,7 +5133,7 @@
         <v>MWF</v>
       </c>
       <c r="M67" t="str">
-        <v>11:00:00</v>
+        <v>14:45:00</v>
       </c>
       <c r="N67">
         <v>65</v>
@@ -5134,7 +5142,7 @@
         <v>SB 382</v>
       </c>
       <c r="P67" t="str">
-        <v>Artificial Intelligence</v>
+        <v>High Performance Computing</v>
       </c>
       <c r="Q67" t="str">
         <v/>
@@ -5169,13 +5177,13 @@
         <v>SP</v>
       </c>
       <c r="D68" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E68" t="str">
         <v>CS</v>
       </c>
       <c r="F68" t="str">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G68" t="str">
         <v>A</v>
@@ -5205,7 +5213,7 @@
         <v>SB 382</v>
       </c>
       <c r="P68" t="str">
-        <v>Machine Learning</v>
+        <v>Artificial Intelligence</v>
       </c>
       <c r="Q68" t="str">
         <v/>
@@ -5237,46 +5245,46 @@
         <v/>
       </c>
       <c r="C69" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D69" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="E69" t="str">
         <v>CS</v>
       </c>
       <c r="F69" t="str">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="G69" t="str">
         <v>A</v>
       </c>
       <c r="H69" t="str">
-        <v>Derek C Schuurman</v>
+        <v>Kenneth C Arnold</v>
       </c>
       <c r="I69" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J69" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K69" t="str">
         <v/>
       </c>
       <c r="L69" t="str">
-        <v>R</v>
+        <v>MWF</v>
       </c>
       <c r="M69" t="str">
-        <v>19:00:00</v>
+        <v>11:00:00</v>
       </c>
       <c r="N69">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O69" t="str">
         <v>SB 382</v>
       </c>
       <c r="P69" t="str">
-        <v>Senior Internship in Computing</v>
+        <v>Machine Learning</v>
       </c>
       <c r="Q69" t="str">
         <v/>
@@ -5308,7 +5316,7 @@
         <v/>
       </c>
       <c r="C70" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D70" t="str">
         <v>Full</v>
@@ -5388,7 +5396,7 @@
         <v>CS</v>
       </c>
       <c r="F71" t="str">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G71" t="str">
         <v>A</v>
@@ -5397,28 +5405,28 @@
         <v>Derek C Schuurman</v>
       </c>
       <c r="I71" t="str">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J71" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K71" t="str">
         <v/>
       </c>
       <c r="L71" t="str">
-        <v>TR</v>
+        <v>R</v>
       </c>
       <c r="M71" t="str">
-        <v>10:20:00</v>
+        <v>19:00:00</v>
       </c>
       <c r="N71">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O71" t="str">
-        <v>SC 203</v>
+        <v>SB 382</v>
       </c>
       <c r="P71" t="str">
-        <v>Perspectives on Computing</v>
+        <v>Senior Internship in Computing</v>
       </c>
       <c r="Q71" t="str">
         <v/>
@@ -5462,7 +5470,7 @@
         <v>384</v>
       </c>
       <c r="G72" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="H72" t="str">
         <v>Derek C Schuurman</v>
@@ -5480,7 +5488,7 @@
         <v>TR</v>
       </c>
       <c r="M72" t="str">
-        <v>12:15:00</v>
+        <v>10:20:00</v>
       </c>
       <c r="N72">
         <v>100</v>
@@ -5521,7 +5529,7 @@
         <v/>
       </c>
       <c r="C73" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D73" t="str">
         <v>Full</v>
@@ -5530,37 +5538,37 @@
         <v>CS</v>
       </c>
       <c r="F73" t="str">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="G73" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="H73" t="str">
-        <v>Kenneth C Arnold</v>
+        <v>Derek C Schuurman</v>
       </c>
       <c r="I73" t="str">
-        <v>0.3</v>
+        <v>4</v>
       </c>
       <c r="J73" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K73" t="str">
         <v/>
       </c>
       <c r="L73" t="str">
-        <v>T</v>
+        <v>TR</v>
       </c>
       <c r="M73" t="str">
-        <v>19:00:00</v>
+        <v>12:15:00</v>
       </c>
       <c r="N73">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O73" t="str">
-        <v>SB 382</v>
+        <v>SC 203</v>
       </c>
       <c r="P73" t="str">
-        <v>Senior Project in Computing I</v>
+        <v>Perspectives on Computing</v>
       </c>
       <c r="Q73" t="str">
         <v/>
@@ -5592,7 +5600,7 @@
         <v/>
       </c>
       <c r="C74" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D74" t="str">
         <v>Full</v>
@@ -5601,7 +5609,7 @@
         <v>CS</v>
       </c>
       <c r="F74" t="str">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G74" t="str">
         <v>A</v>
@@ -5631,7 +5639,7 @@
         <v>SB 382</v>
       </c>
       <c r="P74" t="str">
-        <v>Senior Project in Computing II</v>
+        <v>Senior Project in Computing I</v>
       </c>
       <c r="Q74" t="str">
         <v/>
@@ -5663,25 +5671,25 @@
         <v/>
       </c>
       <c r="C75" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D75" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="E75" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="F75" t="str">
-        <v>102</v>
+        <v>398</v>
       </c>
       <c r="G75" t="str">
         <v>A</v>
       </c>
       <c r="H75" t="str">
-        <v>Jim Momeyer</v>
+        <v>Kenneth C Arnold</v>
       </c>
       <c r="I75" t="str">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="J75" t="str">
         <v>2</v>
@@ -5690,25 +5698,25 @@
         <v/>
       </c>
       <c r="L75" t="str">
-        <v>TR</v>
+        <v>T</v>
       </c>
       <c r="M75" t="str">
-        <v>08:00:00</v>
+        <v>19:00:00</v>
       </c>
       <c r="N75">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O75" t="str">
-        <v>SB 354</v>
+        <v>SB 382</v>
       </c>
       <c r="P75" t="str">
-        <v>Foundations of Data Science and Analytics</v>
+        <v>Senior Project in Computing II</v>
       </c>
       <c r="Q75" t="str">
         <v/>
       </c>
       <c r="R75" t="str">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="S75" t="str">
         <v/>
@@ -5726,7 +5734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" xml:space="preserve">
+    <row r="76">
       <c r="A76" t="str">
         <v>Computer Science</v>
       </c>
@@ -5734,7 +5742,7 @@
         <v/>
       </c>
       <c r="C76" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D76" t="str">
         <v>First</v>
@@ -5749,7 +5757,7 @@
         <v>A</v>
       </c>
       <c r="H76" t="str">
-        <v>Fernando Pasquini Santos</v>
+        <v>Jim Momeyer</v>
       </c>
       <c r="I76" t="str">
         <v>2</v>
@@ -5761,13 +5769,13 @@
         <v/>
       </c>
       <c r="L76" t="str">
-        <v>MWF</v>
+        <v>TR</v>
       </c>
       <c r="M76" t="str">
-        <v>09:15:00</v>
+        <v>08:00:00</v>
       </c>
       <c r="N76">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O76" t="str">
         <v>SB 354</v>
@@ -5787,9 +5795,8 @@
       <c r="T76" t="str">
         <v/>
       </c>
-      <c r="U76" t="str" xml:space="preserve">
-        <v xml:space="preserve">Monica is busy with ENGR labs all day Thursday.
-Set as on-hold? we may not have the enrollment.</v>
+      <c r="U76" t="str">
+        <v/>
       </c>
       <c r="V76">
         <v>0</v>
@@ -6295,7 +6302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" xml:space="preserve">
+    <row r="84">
       <c r="A84" t="str">
         <v>Computer Science</v>
       </c>
@@ -6303,7 +6310,7 @@
         <v/>
       </c>
       <c r="C84" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D84" t="str">
         <v>Second</v>
@@ -6315,10 +6322,10 @@
         <v>102</v>
       </c>
       <c r="G84" t="str">
-        <v>E</v>
+        <v>F</v>
       </c>
       <c r="H84" t="str">
-        <v>Fernando Pasquini Santos</v>
+        <v>Cancelled-DATA</v>
       </c>
       <c r="I84" t="str">
         <v>2</v>
@@ -6330,13 +6337,13 @@
         <v/>
       </c>
       <c r="L84" t="str">
-        <v>MWF</v>
+        <v>TR</v>
       </c>
       <c r="M84" t="str">
-        <v>09:15:00</v>
+        <v>12:15:00</v>
       </c>
       <c r="N84">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O84" t="str">
         <v>SB 354</v>
@@ -6356,9 +6363,8 @@
       <c r="T84" t="str">
         <v/>
       </c>
-      <c r="U84" t="str" xml:space="preserve">
-        <v xml:space="preserve">Monica is busy with ENGR labs all day Thursday.
-Set as on-hold? we may not have the enrollment.</v>
+      <c r="U84" t="str">
+        <v/>
       </c>
       <c r="V84">
         <v>0</v>
@@ -6375,7 +6381,7 @@
         <v/>
       </c>
       <c r="C85" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D85" t="str">
         <v>Second</v>
@@ -6446,7 +6452,7 @@
         <v/>
       </c>
       <c r="C86" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D86" t="str">
         <v>Second</v>
@@ -6458,7 +6464,7 @@
         <v>102</v>
       </c>
       <c r="G86" t="str">
-        <v>F</v>
+        <v>G</v>
       </c>
       <c r="H86" t="str">
         <v>Cancelled-DATA</v>
@@ -6476,7 +6482,7 @@
         <v>TR</v>
       </c>
       <c r="M86" t="str">
-        <v>12:15:00</v>
+        <v>14:10:00</v>
       </c>
       <c r="N86">
         <v>100</v>
@@ -6517,7 +6523,7 @@
         <v/>
       </c>
       <c r="C87" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D87" t="str">
         <v>Second</v>
@@ -6588,7 +6594,7 @@
         <v/>
       </c>
       <c r="C88" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D88" t="str">
         <v>Second</v>
@@ -6600,10 +6606,10 @@
         <v>102</v>
       </c>
       <c r="G88" t="str">
-        <v>G</v>
+        <v>H</v>
       </c>
       <c r="H88" t="str">
-        <v>Cancelled-DATA</v>
+        <v>Jim Momeyer</v>
       </c>
       <c r="I88" t="str">
         <v>2</v>
@@ -6618,7 +6624,7 @@
         <v>TR</v>
       </c>
       <c r="M88" t="str">
-        <v>14:10:00</v>
+        <v>19:00:00</v>
       </c>
       <c r="N88">
         <v>100</v>
@@ -6659,7 +6665,7 @@
         <v/>
       </c>
       <c r="C89" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D89" t="str">
         <v>Second</v>
@@ -6722,7 +6728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" xml:space="preserve">
       <c r="A90" t="str">
         <v>Computer Science</v>
       </c>
@@ -6733,7 +6739,7 @@
         <v>SP</v>
       </c>
       <c r="D90" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E90" t="str">
         <v>DATA</v>
@@ -6742,7 +6748,7 @@
         <v>102</v>
       </c>
       <c r="G90" t="str">
-        <v>H</v>
+        <v>A</v>
       </c>
       <c r="H90" t="str">
         <v>Jim Momeyer</v>
@@ -6757,13 +6763,13 @@
         <v/>
       </c>
       <c r="L90" t="str">
-        <v>TR</v>
+        <v>MWF</v>
       </c>
       <c r="M90" t="str">
-        <v>19:00:00</v>
+        <v>09:15:00</v>
       </c>
       <c r="N90">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="O90" t="str">
         <v>SB 354</v>
@@ -6783,8 +6789,9 @@
       <c r="T90" t="str">
         <v/>
       </c>
-      <c r="U90" t="str">
-        <v/>
+      <c r="U90" t="str" xml:space="preserve">
+        <v xml:space="preserve">Monica is busy with ENGR labs all day Thursday.
+Set as on-hold? we may not have the enrollment.</v>
       </c>
       <c r="V90">
         <v>0</v>
@@ -6793,7 +6800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" xml:space="preserve">
       <c r="A91" t="str">
         <v>Computer Science</v>
       </c>
@@ -6801,28 +6808,28 @@
         <v/>
       </c>
       <c r="C91" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D91" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="E91" t="str">
         <v>DATA</v>
       </c>
       <c r="F91" t="str">
-        <v>202</v>
+        <v>102</v>
       </c>
       <c r="G91" t="str">
-        <v>A</v>
+        <v>E</v>
       </c>
       <c r="H91" t="str">
-        <v>Fernando Pasquini Santos</v>
+        <v>Jim Momeyer</v>
       </c>
       <c r="I91" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J91" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K91" t="str">
         <v/>
@@ -6831,22 +6838,22 @@
         <v>MWF</v>
       </c>
       <c r="M91" t="str">
-        <v>08:00:00</v>
+        <v>09:15:00</v>
       </c>
       <c r="N91">
         <v>65</v>
       </c>
       <c r="O91" t="str">
-        <v>SB 382</v>
+        <v>SB 354</v>
       </c>
       <c r="P91" t="str">
-        <v>Predictive Analytics</v>
+        <v>Foundations of Data Science and Analytics</v>
       </c>
       <c r="Q91" t="str">
         <v/>
       </c>
       <c r="R91" t="str">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="S91" t="str">
         <v/>
@@ -6854,8 +6861,9 @@
       <c r="T91" t="str">
         <v/>
       </c>
-      <c r="U91" t="str">
-        <v/>
+      <c r="U91" t="str" xml:space="preserve">
+        <v xml:space="preserve">Monica is busy with ENGR labs all day Thursday.
+Set as on-hold? we may not have the enrollment.</v>
       </c>
       <c r="V91">
         <v>0</v>
@@ -6884,7 +6892,7 @@
         <v>202</v>
       </c>
       <c r="G92" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="H92" t="str">
         <v>Fernando Pasquini Santos</v>
@@ -6902,7 +6910,7 @@
         <v>MWF</v>
       </c>
       <c r="M92" t="str">
-        <v>09:15:00</v>
+        <v>08:00:00</v>
       </c>
       <c r="N92">
         <v>65</v>
@@ -6952,43 +6960,43 @@
         <v>DATA</v>
       </c>
       <c r="F93" t="str">
-        <v>396</v>
+        <v>202</v>
       </c>
       <c r="G93" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="H93" t="str">
-        <v>Kenneth C Arnold</v>
+        <v>Fernando Pasquini Santos</v>
       </c>
       <c r="I93" t="str">
-        <v>0.3</v>
+        <v>4</v>
       </c>
       <c r="J93" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K93" t="str">
         <v/>
       </c>
       <c r="L93" t="str">
-        <v>T</v>
+        <v>MWF</v>
       </c>
       <c r="M93" t="str">
-        <v>19:00:00</v>
+        <v>09:15:00</v>
       </c>
       <c r="N93">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O93" t="str">
         <v>SB 382</v>
       </c>
       <c r="P93" t="str">
-        <v>Senior Project in Data Science</v>
+        <v>Predictive Analytics</v>
       </c>
       <c r="Q93" t="str">
         <v/>
       </c>
       <c r="R93" t="str">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="S93" t="str">
         <v/>
@@ -7014,7 +7022,7 @@
         <v/>
       </c>
       <c r="C94" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D94" t="str">
         <v>Full</v>
@@ -7023,7 +7031,7 @@
         <v>DATA</v>
       </c>
       <c r="F94" t="str">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G94" t="str">
         <v>A</v>
@@ -7053,7 +7061,7 @@
         <v>SB 382</v>
       </c>
       <c r="P94" t="str">
-        <v>Senior Project in Data Science II</v>
+        <v>Senior Project in Data Science</v>
       </c>
       <c r="Q94" t="str">
         <v/>
@@ -7085,25 +7093,25 @@
         <v/>
       </c>
       <c r="C95" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D95" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="E95" t="str">
         <v>DATA</v>
       </c>
       <c r="F95" t="str">
-        <v>501</v>
+        <v>398</v>
       </c>
       <c r="G95" t="str">
         <v>A</v>
       </c>
       <c r="H95" t="str">
-        <v>Cancelled-MDS</v>
+        <v>Kenneth C Arnold</v>
       </c>
       <c r="I95" t="str">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="J95" t="str">
         <v>2</v>
@@ -7112,25 +7120,25 @@
         <v/>
       </c>
       <c r="L95" t="str">
-        <v/>
+        <v>T</v>
       </c>
       <c r="M95" t="str">
-        <v/>
-      </c>
-      <c r="N95" t="str">
-        <v/>
+        <v>19:00:00</v>
+      </c>
+      <c r="N95">
+        <v>50</v>
       </c>
       <c r="O95" t="str">
-        <v/>
+        <v>SB 382</v>
       </c>
       <c r="P95" t="str">
-        <v>Data Wrangling</v>
+        <v>Senior Project in Data Science II</v>
       </c>
       <c r="Q95" t="str">
         <v/>
       </c>
       <c r="R95" t="str">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="S95" t="str">
         <v/>
@@ -7159,13 +7167,13 @@
         <v>FA</v>
       </c>
       <c r="D96" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E96" t="str">
         <v>DATA</v>
       </c>
       <c r="F96" t="str">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G96" t="str">
         <v>A</v>
@@ -7195,7 +7203,7 @@
         <v/>
       </c>
       <c r="P96" t="str">
-        <v>Introduction to Machine Learning</v>
+        <v>Data Wrangling</v>
       </c>
       <c r="Q96" t="str">
         <v/>
@@ -7227,16 +7235,16 @@
         <v/>
       </c>
       <c r="C97" t="str">
-        <v>SU</v>
+        <v>FA</v>
       </c>
       <c r="D97" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="E97" t="str">
         <v>DATA</v>
       </c>
       <c r="F97" t="str">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="G97" t="str">
         <v>A</v>
@@ -7266,7 +7274,7 @@
         <v/>
       </c>
       <c r="P97" t="str">
-        <v>Visualization for Data Science</v>
+        <v>Introduction to Machine Learning</v>
       </c>
       <c r="Q97" t="str">
         <v/>
@@ -7298,7 +7306,7 @@
         <v/>
       </c>
       <c r="C98" t="str">
-        <v>SP</v>
+        <v>SU</v>
       </c>
       <c r="D98" t="str">
         <v>First</v>
@@ -7307,7 +7315,7 @@
         <v>DATA</v>
       </c>
       <c r="F98" t="str">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="G98" t="str">
         <v>A</v>
@@ -7337,7 +7345,7 @@
         <v/>
       </c>
       <c r="P98" t="str">
-        <v>Ethics for Data Science</v>
+        <v>Visualization for Data Science</v>
       </c>
       <c r="Q98" t="str">
         <v/>
@@ -7369,16 +7377,16 @@
         <v/>
       </c>
       <c r="C99" t="str">
-        <v>SU</v>
+        <v>SP</v>
       </c>
       <c r="D99" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E99" t="str">
         <v>DATA</v>
       </c>
       <c r="F99" t="str">
-        <v>539</v>
+        <v>510</v>
       </c>
       <c r="G99" t="str">
         <v>A</v>
@@ -7408,7 +7416,7 @@
         <v/>
       </c>
       <c r="P99" t="str">
-        <v>Administering Cloud Services</v>
+        <v>Ethics for Data Science</v>
       </c>
       <c r="Q99" t="str">
         <v/>
@@ -7440,16 +7448,16 @@
         <v/>
       </c>
       <c r="C100" t="str">
-        <v>SP</v>
+        <v>SU</v>
       </c>
       <c r="D100" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="E100" t="str">
         <v>DATA</v>
       </c>
       <c r="F100" t="str">
-        <v>562</v>
+        <v>539</v>
       </c>
       <c r="G100" t="str">
         <v>A</v>
@@ -7458,10 +7466,10 @@
         <v>Cancelled-MDS</v>
       </c>
       <c r="I100" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J100" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K100" t="str">
         <v/>
@@ -7479,7 +7487,7 @@
         <v/>
       </c>
       <c r="P100" t="str">
-        <v>Systems Engineering for Data Science</v>
+        <v>Administering Cloud Services</v>
       </c>
       <c r="Q100" t="str">
         <v/>
@@ -7511,16 +7519,16 @@
         <v/>
       </c>
       <c r="C101" t="str">
-        <v>SU</v>
+        <v>SP</v>
       </c>
       <c r="D101" t="str">
-        <v>Second</v>
+        <v>Full</v>
       </c>
       <c r="E101" t="str">
         <v>DATA</v>
       </c>
       <c r="F101" t="str">
-        <v>654</v>
+        <v>562</v>
       </c>
       <c r="G101" t="str">
         <v>A</v>
@@ -7529,10 +7537,10 @@
         <v>Cancelled-MDS</v>
       </c>
       <c r="I101" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J101" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K101" t="str">
         <v/>
@@ -7550,13 +7558,13 @@
         <v/>
       </c>
       <c r="P101" t="str">
-        <v>Database Management Systems</v>
+        <v>Systems Engineering for Data Science</v>
       </c>
       <c r="Q101" t="str">
         <v/>
       </c>
       <c r="R101" t="str">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="S101" t="str">
         <v/>
@@ -7582,7 +7590,7 @@
         <v/>
       </c>
       <c r="C102" t="str">
-        <v>SP</v>
+        <v>SU</v>
       </c>
       <c r="D102" t="str">
         <v>Second</v>
@@ -7591,7 +7599,7 @@
         <v>DATA</v>
       </c>
       <c r="F102" t="str">
-        <v>675</v>
+        <v>654</v>
       </c>
       <c r="G102" t="str">
         <v>A</v>
@@ -7621,7 +7629,7 @@
         <v/>
       </c>
       <c r="P102" t="str">
-        <v>Introduction to Deep Learning</v>
+        <v>Database Management Systems</v>
       </c>
       <c r="Q102" t="str">
         <v/>
@@ -7653,16 +7661,16 @@
         <v/>
       </c>
       <c r="C103" t="str">
-        <v>SU</v>
+        <v>SP</v>
       </c>
       <c r="D103" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="E103" t="str">
         <v>DATA</v>
       </c>
       <c r="F103" t="str">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G103" t="str">
         <v>A</v>
@@ -7692,7 +7700,7 @@
         <v/>
       </c>
       <c r="P103" t="str">
-        <v>Deep Learning for Text and Generative Models</v>
+        <v>Introduction to Deep Learning</v>
       </c>
       <c r="Q103" t="str">
         <v/>
@@ -7727,13 +7735,13 @@
         <v>SU</v>
       </c>
       <c r="D104" t="str">
-        <v>Full</v>
+        <v>First</v>
       </c>
       <c r="E104" t="str">
         <v>DATA</v>
       </c>
       <c r="F104" t="str">
-        <v>696</v>
+        <v>676</v>
       </c>
       <c r="G104" t="str">
         <v>A</v>
@@ -7763,7 +7771,7 @@
         <v/>
       </c>
       <c r="P104" t="str">
-        <v>Project in Data Science</v>
+        <v>Deep Learning for Text and Generative Models</v>
       </c>
       <c r="Q104" t="str">
         <v/>
@@ -7798,13 +7806,13 @@
         <v>SU</v>
       </c>
       <c r="D105" t="str">
-        <v>Second</v>
+        <v>Full</v>
       </c>
       <c r="E105" t="str">
         <v>DATA</v>
       </c>
       <c r="F105" t="str">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="G105" t="str">
         <v>A</v>
@@ -7866,22 +7874,22 @@
         <v/>
       </c>
       <c r="C106" t="str">
-        <v>FA</v>
+        <v>SU</v>
       </c>
       <c r="D106" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="E106" t="str">
-        <v>HNRS</v>
+        <v>DATA</v>
       </c>
       <c r="F106" t="str">
-        <v>251</v>
+        <v>698</v>
       </c>
       <c r="G106" t="str">
         <v>A</v>
       </c>
       <c r="H106" t="str">
-        <v>Eric Araujo</v>
+        <v>Cancelled-MDS</v>
       </c>
       <c r="I106" t="str">
         <v>2</v>
@@ -7893,25 +7901,25 @@
         <v/>
       </c>
       <c r="L106" t="str">
-        <v>TR</v>
+        <v/>
       </c>
       <c r="M106" t="str">
-        <v>14:10:00</v>
-      </c>
-      <c r="N106">
-        <v>65</v>
+        <v/>
+      </c>
+      <c r="N106" t="str">
+        <v/>
       </c>
       <c r="O106" t="str">
-        <v>HL 406C</v>
+        <v/>
       </c>
       <c r="P106" t="str">
-        <v>Agent Modeling</v>
+        <v>Project in Data Science</v>
       </c>
       <c r="Q106" t="str">
         <v/>
       </c>
       <c r="R106" t="str">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="S106" t="str">
         <v/>
@@ -7931,7 +7939,7 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>Shadow</v>
+        <v>Computer Science</v>
       </c>
       <c r="B107" t="str">
         <v/>
@@ -7940,49 +7948,49 @@
         <v>FA</v>
       </c>
       <c r="D107" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="E107" t="str">
-        <v>CS</v>
+        <v>HNRS</v>
       </c>
       <c r="F107" t="str">
-        <v>300-S</v>
+        <v>251</v>
       </c>
       <c r="G107" t="str">
-        <v>A-S</v>
+        <v>A</v>
       </c>
       <c r="H107" t="str">
-        <v>Shadow-Gold</v>
+        <v>Eric Araujo</v>
       </c>
       <c r="I107" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J107" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K107" t="str">
         <v/>
       </c>
       <c r="L107" t="str">
-        <v>MWF</v>
+        <v>TR</v>
       </c>
       <c r="M107" t="str">
-        <v>11:00:00</v>
+        <v>14:10:00</v>
       </c>
       <c r="N107">
         <v>65</v>
       </c>
       <c r="O107" t="str">
-        <v>SB 354</v>
+        <v>HL 406C</v>
       </c>
       <c r="P107" t="str">
-        <v>Applied Machine Learning</v>
+        <v>Agent Modeling</v>
       </c>
       <c r="Q107" t="str">
         <v/>
       </c>
       <c r="R107" t="str">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="S107" t="str">
         <v/>
@@ -8008,10 +8016,10 @@
         <v/>
       </c>
       <c r="C108" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D108" t="str">
-        <v>Full</v>
+        <v>First</v>
       </c>
       <c r="E108" t="str">
         <v>CS</v>
@@ -8038,7 +8046,7 @@
         <v>MWF</v>
       </c>
       <c r="M108" t="str">
-        <v>12:15:00</v>
+        <v>11:00:00</v>
       </c>
       <c r="N108">
         <v>65</v>
@@ -8079,10 +8087,10 @@
         <v/>
       </c>
       <c r="C109" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D109" t="str">
-        <v>Second</v>
+        <v>Full</v>
       </c>
       <c r="E109" t="str">
         <v>CS</v>
@@ -8091,7 +8099,7 @@
         <v>300-S</v>
       </c>
       <c r="G109" t="str">
-        <v>B-S</v>
+        <v>A-S</v>
       </c>
       <c r="H109" t="str">
         <v>Shadow-Gold</v>
@@ -8109,7 +8117,7 @@
         <v>MWF</v>
       </c>
       <c r="M109" t="str">
-        <v>11:00:00</v>
+        <v>12:15:00</v>
       </c>
       <c r="N109">
         <v>65</v>
@@ -8150,19 +8158,19 @@
         <v/>
       </c>
       <c r="C110" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D110" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="E110" t="str">
         <v>CS</v>
       </c>
       <c r="F110" t="str">
-        <v>338-S</v>
+        <v>300-S</v>
       </c>
       <c r="G110" t="str">
-        <v>A-S</v>
+        <v>B-S</v>
       </c>
       <c r="H110" t="str">
         <v>Shadow-Gold</v>
@@ -8180,7 +8188,7 @@
         <v>MWF</v>
       </c>
       <c r="M110" t="str">
-        <v>08:00:00</v>
+        <v>11:00:00</v>
       </c>
       <c r="N110">
         <v>65</v>
@@ -8189,7 +8197,7 @@
         <v>SB 354</v>
       </c>
       <c r="P110" t="str">
-        <v>System Administration: Infrastructure</v>
+        <v>Applied Machine Learning</v>
       </c>
       <c r="Q110" t="str">
         <v/>
@@ -8224,13 +8232,13 @@
         <v>SP</v>
       </c>
       <c r="D111" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E111" t="str">
         <v>CS</v>
       </c>
       <c r="F111" t="str">
-        <v>339-S</v>
+        <v>338-S</v>
       </c>
       <c r="G111" t="str">
         <v>A-S</v>
@@ -8260,7 +8268,7 @@
         <v>SB 354</v>
       </c>
       <c r="P111" t="str">
-        <v>System Administration: Cloud Services</v>
+        <v>System Administration: Infrastructure</v>
       </c>
       <c r="Q111" t="str">
         <v/>
@@ -8292,7 +8300,7 @@
         <v/>
       </c>
       <c r="C112" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D112" t="str">
         <v>Second</v>
@@ -8301,7 +8309,7 @@
         <v>CS</v>
       </c>
       <c r="F112" t="str">
-        <v>374-S</v>
+        <v>339-S</v>
       </c>
       <c r="G112" t="str">
         <v>A-S</v>
@@ -8310,19 +8318,19 @@
         <v>Shadow-Gold</v>
       </c>
       <c r="I112" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J112" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K112" t="str">
         <v/>
       </c>
       <c r="L112" t="str">
-        <v>MW</v>
+        <v>MWF</v>
       </c>
       <c r="M112" t="str">
-        <v>14:45:00</v>
+        <v>08:00:00</v>
       </c>
       <c r="N112">
         <v>65</v>
@@ -8331,7 +8339,7 @@
         <v>SB 354</v>
       </c>
       <c r="P112" t="str">
-        <v>High-Performance Computing</v>
+        <v>System Administration: Cloud Services</v>
       </c>
       <c r="Q112" t="str">
         <v/>
@@ -8363,16 +8371,16 @@
         <v/>
       </c>
       <c r="C113" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D113" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="E113" t="str">
         <v>CS</v>
       </c>
       <c r="F113" t="str">
-        <v>375-S</v>
+        <v>374-S</v>
       </c>
       <c r="G113" t="str">
         <v>A-S</v>
@@ -8381,19 +8389,19 @@
         <v>Shadow-Gold</v>
       </c>
       <c r="I113" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J113" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K113" t="str">
         <v/>
       </c>
       <c r="L113" t="str">
-        <v>MWF</v>
+        <v>MW</v>
       </c>
       <c r="M113" t="str">
-        <v>11:00:00</v>
+        <v>14:45:00</v>
       </c>
       <c r="N113">
         <v>65</v>
@@ -8402,7 +8410,7 @@
         <v>SB 354</v>
       </c>
       <c r="P113" t="str">
-        <v>Artificial Intelligence</v>
+        <v>High-Performance Computing</v>
       </c>
       <c r="Q113" t="str">
         <v/>
@@ -8437,16 +8445,16 @@
         <v>SP</v>
       </c>
       <c r="D114" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E114" t="str">
         <v>CS</v>
       </c>
       <c r="F114" t="str">
-        <v>376-S</v>
+        <v>375-S</v>
       </c>
       <c r="G114" t="str">
-        <v>B-S</v>
+        <v>A-S</v>
       </c>
       <c r="H114" t="str">
         <v>Shadow-Gold</v>
@@ -8473,7 +8481,7 @@
         <v>SB 354</v>
       </c>
       <c r="P114" t="str">
-        <v>Machine Learning</v>
+        <v>Artificial Intelligence</v>
       </c>
       <c r="Q114" t="str">
         <v/>
@@ -8505,22 +8513,22 @@
         <v/>
       </c>
       <c r="C115" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D115" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="E115" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="F115" t="str">
-        <v>202-S</v>
+        <v>376-S</v>
       </c>
       <c r="G115" t="str">
-        <v>A-S</v>
+        <v>B-S</v>
       </c>
       <c r="H115" t="str">
-        <v>Shadow-Maroon</v>
+        <v>Shadow-Gold</v>
       </c>
       <c r="I115" t="str">
         <v>0</v>
@@ -8535,7 +8543,7 @@
         <v>MWF</v>
       </c>
       <c r="M115" t="str">
-        <v>08:00:00</v>
+        <v>11:00:00</v>
       </c>
       <c r="N115">
         <v>65</v>
@@ -8544,13 +8552,13 @@
         <v>SB 354</v>
       </c>
       <c r="P115" t="str">
-        <v>Predictive Analytics</v>
+        <v>Machine Learning</v>
       </c>
       <c r="Q115" t="str">
         <v/>
       </c>
       <c r="R115" t="str">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="S115" t="str">
         <v/>
@@ -8588,7 +8596,7 @@
         <v>202-S</v>
       </c>
       <c r="G116" t="str">
-        <v>B-S</v>
+        <v>A-S</v>
       </c>
       <c r="H116" t="str">
         <v>Shadow-Maroon</v>
@@ -8606,7 +8614,7 @@
         <v>MWF</v>
       </c>
       <c r="M116" t="str">
-        <v>09:15:00</v>
+        <v>08:00:00</v>
       </c>
       <c r="N116">
         <v>65</v>
@@ -8641,7 +8649,7 @@
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>Computer Science</v>
+        <v>Shadow</v>
       </c>
       <c r="B117" t="str">
         <v/>
@@ -8653,46 +8661,46 @@
         <v>Full</v>
       </c>
       <c r="E117" t="str">
-        <v>CS</v>
+        <v>DATA</v>
       </c>
       <c r="F117" t="str">
-        <v>364</v>
+        <v>202-S</v>
       </c>
       <c r="G117" t="str">
-        <v>A</v>
+        <v>B-S</v>
       </c>
       <c r="H117" t="str">
-        <v>Brian D Paige</v>
+        <v>Shadow-Maroon</v>
       </c>
       <c r="I117" t="str">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J117" t="str">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K117" t="str">
         <v/>
       </c>
       <c r="L117" t="str">
-        <v>MR</v>
+        <v>MWF</v>
       </c>
       <c r="M117" t="str">
-        <v>19:00:00</v>
+        <v>09:15:00</v>
       </c>
       <c r="N117">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="O117" t="str">
-        <v>SB 372</v>
+        <v>SB 354</v>
       </c>
       <c r="P117" t="str">
-        <v>Computer Security</v>
+        <v>Predictive Analytics</v>
       </c>
       <c r="Q117" t="str">
         <v/>
       </c>
       <c r="R117" t="str">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="S117" t="str">
         <v/>
@@ -9675,7 +9683,7 @@
         <v/>
       </c>
     </row>
-    <row r="19">
+    <row r="19" xml:space="preserve">
       <c r="A19" t="str">
         <v>FA</v>
       </c>
@@ -9694,14 +9702,16 @@
       <c r="F19" t="str">
         <v>0</v>
       </c>
-      <c r="G19" t="str">
-        <v>MTWRF</v>
+      <c r="G19" t="str" xml:space="preserve">
+        <v xml:space="preserve">MTWRF
+MWF
+TR</v>
       </c>
       <c r="H19" t="str">
         <v>16:00:00 - 18:15:00</v>
       </c>
       <c r="I19" t="str">
-        <v>, ,</v>
+        <v xml:space="preserve">, , </v>
       </c>
       <c r="J19" t="str">
         <v>Full</v>
@@ -9728,7 +9738,7 @@
         <v/>
       </c>
     </row>
-    <row r="20">
+    <row r="20" xml:space="preserve">
       <c r="A20" t="str">
         <v>SP</v>
       </c>
@@ -9747,14 +9757,16 @@
       <c r="F20" t="str">
         <v>0</v>
       </c>
-      <c r="G20" t="str">
-        <v>MTWRF</v>
+      <c r="G20" t="str" xml:space="preserve">
+        <v xml:space="preserve">MTWRF
+MWF
+TR</v>
       </c>
       <c r="H20" t="str">
         <v>16:00:00 - 18:15:00</v>
       </c>
       <c r="I20" t="str">
-        <v>, ,</v>
+        <v xml:space="preserve">, , </v>
       </c>
       <c r="J20" t="str">
         <v>Full</v>
@@ -10458,7 +10470,7 @@
         <v>Intro to Computing</v>
       </c>
       <c r="N33" t="str">
-        <v>Keith VanderLinden</v>
+        <v>Fernando Pasquini Santos</v>
       </c>
       <c r="O33" t="str">
         <v/>
@@ -11318,7 +11330,7 @@
         <v/>
       </c>
     </row>
-    <row r="50">
+    <row r="50" xml:space="preserve">
       <c r="A50" t="str">
         <v>SP</v>
       </c>
@@ -11337,8 +11349,9 @@
       <c r="F50" t="str">
         <v>4</v>
       </c>
-      <c r="G50" t="str">
-        <v>MW</v>
+      <c r="G50" t="str" xml:space="preserve">
+        <v xml:space="preserve">MW
+F</v>
       </c>
       <c r="H50" t="str">
         <v>14:45:00 - 15:50:00</v>
@@ -11371,7 +11384,7 @@
         <v/>
       </c>
     </row>
-    <row r="51">
+    <row r="51" xml:space="preserve">
       <c r="A51" t="str">
         <v>SP</v>
       </c>
@@ -11390,8 +11403,9 @@
       <c r="F51" t="str">
         <v>4</v>
       </c>
-      <c r="G51" t="str">
-        <v>F</v>
+      <c r="G51" t="str" xml:space="preserve">
+        <v xml:space="preserve">F
+MW</v>
       </c>
       <c r="H51" t="str">
         <v>14:45:00 - 17:05:00</v>
@@ -11450,7 +11464,7 @@
         <v>08:00:00 - 09:05:00</v>
       </c>
       <c r="I52" t="str">
-        <v>SB 372</v>
+        <v>NH 64</v>
       </c>
       <c r="J52" t="str">
         <v>Full</v>
@@ -11530,7 +11544,7 @@
         <v/>
       </c>
     </row>
-    <row r="54">
+    <row r="54" xml:space="preserve">
       <c r="A54" t="str">
         <v>FA</v>
       </c>
@@ -11549,8 +11563,9 @@
       <c r="F54" t="str">
         <v>4</v>
       </c>
-      <c r="G54" t="str">
-        <v>F</v>
+      <c r="G54" t="str" xml:space="preserve">
+        <v xml:space="preserve">F
+MW</v>
       </c>
       <c r="H54" t="str">
         <v>13:30:00 - 15:50:00</v>
@@ -11583,7 +11598,7 @@
         <v/>
       </c>
     </row>
-    <row r="55">
+    <row r="55" xml:space="preserve">
       <c r="A55" t="str">
         <v>FA</v>
       </c>
@@ -11602,8 +11617,9 @@
       <c r="F55" t="str">
         <v>4</v>
       </c>
-      <c r="G55" t="str">
-        <v>MW</v>
+      <c r="G55" t="str" xml:space="preserve">
+        <v xml:space="preserve">MW
+F</v>
       </c>
       <c r="H55" t="str">
         <v>14:45:00 - 15:50:00</v>
@@ -12083,10 +12099,10 @@
         <v>MWF</v>
       </c>
       <c r="H64" t="str">
-        <v>09:15:00 - 10:20:00</v>
+        <v>13:30:00 - 14:35:00</v>
       </c>
       <c r="I64" t="str">
-        <v>SB 382</v>
+        <v>SB 372</v>
       </c>
       <c r="J64" t="str">
         <v>Second</v>
@@ -12115,46 +12131,46 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B65" t="str">
         <v>CS</v>
       </c>
       <c r="C65" t="str">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="D65" t="str">
         <v>A</v>
       </c>
       <c r="E65" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F65" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G65" t="str">
-        <v>MWF</v>
+        <v>MR</v>
       </c>
       <c r="H65" t="str">
-        <v>09:15:00 - 10:20:00</v>
+        <v>19:00:00 - 20:40:00</v>
       </c>
       <c r="I65" t="str">
-        <v>SB 382</v>
+        <v>SB 372</v>
       </c>
       <c r="J65" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="K65" t="str">
-        <v>SP-First</v>
+        <v>FA-Full</v>
       </c>
       <c r="L65">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="M65" t="str">
-        <v>Computer Graphics</v>
+        <v>Computer Security</v>
       </c>
       <c r="N65" t="str">
-        <v>Harry Plantinga</v>
+        <v>Brian D Paige, Adam Vedra</v>
       </c>
       <c r="O65" t="str">
         <v/>
@@ -12168,13 +12184,13 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B66" t="str">
         <v>CS</v>
       </c>
       <c r="C66" t="str">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D66" t="str">
         <v>A</v>
@@ -12189,25 +12205,25 @@
         <v>MWF</v>
       </c>
       <c r="H66" t="str">
-        <v>14:45:00 - 15:50:00</v>
+        <v>09:15:00 - 10:20:00</v>
       </c>
       <c r="I66" t="str">
         <v>SB 382</v>
       </c>
       <c r="J66" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="K66" t="str">
-        <v>FA-Second</v>
+        <v>SP-First</v>
       </c>
       <c r="L66">
         <v>65</v>
       </c>
       <c r="M66" t="str">
-        <v>High Performance Computing</v>
+        <v>Computer Graphics</v>
       </c>
       <c r="N66" t="str">
-        <v>Joel Adams</v>
+        <v>Harry Plantinga</v>
       </c>
       <c r="O66" t="str">
         <v/>
@@ -12221,13 +12237,13 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B67" t="str">
         <v>CS</v>
       </c>
       <c r="C67" t="str">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D67" t="str">
         <v>A</v>
@@ -12242,25 +12258,25 @@
         <v>MWF</v>
       </c>
       <c r="H67" t="str">
-        <v>11:00:00 - 12:05:00</v>
+        <v>14:45:00 - 15:50:00</v>
       </c>
       <c r="I67" t="str">
         <v>SB 382</v>
       </c>
       <c r="J67" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="K67" t="str">
-        <v>SP-First</v>
+        <v>FA-Second</v>
       </c>
       <c r="L67">
         <v>65</v>
       </c>
       <c r="M67" t="str">
-        <v>Artificial Intelligence</v>
+        <v>High Performance Computing</v>
       </c>
       <c r="N67" t="str">
-        <v>Kenneth C Arnold</v>
+        <v>Joel Adams</v>
       </c>
       <c r="O67" t="str">
         <v/>
@@ -12280,7 +12296,7 @@
         <v>CS</v>
       </c>
       <c r="C68" t="str">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D68" t="str">
         <v>A</v>
@@ -12301,16 +12317,16 @@
         <v>SB 382</v>
       </c>
       <c r="J68" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="K68" t="str">
-        <v>SP-Second</v>
+        <v>SP-First</v>
       </c>
       <c r="L68">
         <v>65</v>
       </c>
       <c r="M68" t="str">
-        <v>Machine Learning</v>
+        <v>Artificial Intelligence</v>
       </c>
       <c r="N68" t="str">
         <v>Kenneth C Arnold</v>
@@ -12327,46 +12343,46 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B69" t="str">
         <v>CS</v>
       </c>
       <c r="C69" t="str">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="D69" t="str">
         <v>A</v>
       </c>
       <c r="E69" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F69" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G69" t="str">
-        <v>R</v>
+        <v>MWF</v>
       </c>
       <c r="H69" t="str">
-        <v>19:00:00 - 19:50:00</v>
+        <v>11:00:00 - 12:05:00</v>
       </c>
       <c r="I69" t="str">
         <v>SB 382</v>
       </c>
       <c r="J69" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="K69" t="str">
-        <v>FA-Full</v>
+        <v>SP-Second</v>
       </c>
       <c r="L69">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="M69" t="str">
-        <v>Senior Internship in Computing</v>
+        <v>Machine Learning</v>
       </c>
       <c r="N69" t="str">
-        <v>Derek C Schuurman</v>
+        <v>Kenneth C Arnold</v>
       </c>
       <c r="O69" t="str">
         <v/>
@@ -12380,7 +12396,7 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B70" t="str">
         <v>CS</v>
@@ -12410,7 +12426,7 @@
         <v>Full</v>
       </c>
       <c r="K70" t="str">
-        <v>SP-Full</v>
+        <v>FA-Full</v>
       </c>
       <c r="L70">
         <v>50</v>
@@ -12439,25 +12455,25 @@
         <v>CS</v>
       </c>
       <c r="C71" t="str">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D71" t="str">
         <v>A</v>
       </c>
       <c r="E71" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F71" t="str">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G71" t="str">
-        <v>TR</v>
+        <v>R</v>
       </c>
       <c r="H71" t="str">
-        <v>10:20:00 - 12:00:00</v>
+        <v>19:00:00 - 19:50:00</v>
       </c>
       <c r="I71" t="str">
-        <v>SC 203</v>
+        <v>SB 382</v>
       </c>
       <c r="J71" t="str">
         <v>Full</v>
@@ -12466,10 +12482,10 @@
         <v>SP-Full</v>
       </c>
       <c r="L71">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M71" t="str">
-        <v>Perspectives on Computing</v>
+        <v>Senior Internship in Computing</v>
       </c>
       <c r="N71" t="str">
         <v>Derek C Schuurman</v>
@@ -12495,7 +12511,7 @@
         <v>384</v>
       </c>
       <c r="D72" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="E72" t="str">
         <v>4</v>
@@ -12507,7 +12523,7 @@
         <v>TR</v>
       </c>
       <c r="H72" t="str">
-        <v>12:15:00 - 13:55:00</v>
+        <v>10:20:00 - 12:00:00</v>
       </c>
       <c r="I72" t="str">
         <v>SC 203</v>
@@ -12539,46 +12555,46 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B73" t="str">
         <v>CS</v>
       </c>
       <c r="C73" t="str">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="D73" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="E73" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F73" t="str">
-        <v>0.3</v>
+        <v>4</v>
       </c>
       <c r="G73" t="str">
-        <v>T</v>
+        <v>TR</v>
       </c>
       <c r="H73" t="str">
-        <v>19:00:00 - 19:50:00</v>
+        <v>12:15:00 - 13:55:00</v>
       </c>
       <c r="I73" t="str">
-        <v>SB 382</v>
+        <v>SC 203</v>
       </c>
       <c r="J73" t="str">
         <v>Full</v>
       </c>
       <c r="K73" t="str">
-        <v>FA-Full</v>
+        <v>SP-Full</v>
       </c>
       <c r="L73">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M73" t="str">
-        <v>Senior Project in Computing I</v>
+        <v>Perspectives on Computing</v>
       </c>
       <c r="N73" t="str">
-        <v>Kenneth C Arnold</v>
+        <v>Derek C Schuurman</v>
       </c>
       <c r="O73" t="str">
         <v/>
@@ -12592,13 +12608,13 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B74" t="str">
         <v>CS</v>
       </c>
       <c r="C74" t="str">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D74" t="str">
         <v>A</v>
@@ -12622,13 +12638,13 @@
         <v>Full</v>
       </c>
       <c r="K74" t="str">
-        <v>SP-Full</v>
+        <v>FA-Full</v>
       </c>
       <c r="L74">
         <v>50</v>
       </c>
       <c r="M74" t="str">
-        <v>Senior Project in Computing II</v>
+        <v>Senior Project in Computing I</v>
       </c>
       <c r="N74" t="str">
         <v>Kenneth C Arnold</v>
@@ -12645,13 +12661,13 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B75" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="C75" t="str">
-        <v>102</v>
+        <v>398</v>
       </c>
       <c r="D75" t="str">
         <v>A</v>
@@ -12660,31 +12676,31 @@
         <v>2</v>
       </c>
       <c r="F75" t="str">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="G75" t="str">
-        <v>TR</v>
+        <v>T</v>
       </c>
       <c r="H75" t="str">
-        <v>08:00:00 - 09:40:00</v>
+        <v>19:00:00 - 19:50:00</v>
       </c>
       <c r="I75" t="str">
-        <v>SB 354</v>
+        <v>SB 382</v>
       </c>
       <c r="J75" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="K75" t="str">
-        <v>FA-First</v>
+        <v>SP-Full</v>
       </c>
       <c r="L75">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M75" t="str">
-        <v>Foundations of Data Science and Analytics</v>
+        <v>Senior Project in Computing II</v>
       </c>
       <c r="N75" t="str">
-        <v>Jim Momeyer</v>
+        <v>Kenneth C Arnold</v>
       </c>
       <c r="O75" t="str">
         <v/>
@@ -12696,9 +12712,9 @@
         <v/>
       </c>
     </row>
-    <row r="76" xml:space="preserve">
+    <row r="76">
       <c r="A76" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B76" t="str">
         <v>DATA</v>
@@ -12716,10 +12732,10 @@
         <v>2</v>
       </c>
       <c r="G76" t="str">
-        <v>MWF</v>
+        <v>TR</v>
       </c>
       <c r="H76" t="str">
-        <v>09:15:00 - 10:20:00</v>
+        <v>08:00:00 - 09:40:00</v>
       </c>
       <c r="I76" t="str">
         <v>SB 354</v>
@@ -12728,16 +12744,16 @@
         <v>First</v>
       </c>
       <c r="K76" t="str">
-        <v>SP-First</v>
+        <v>FA-First</v>
       </c>
       <c r="L76">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="M76" t="str">
         <v>Foundations of Data Science and Analytics</v>
       </c>
       <c r="N76" t="str">
-        <v>Fernando Pasquini Santos</v>
+        <v>Jim Momeyer</v>
       </c>
       <c r="O76" t="str">
         <v/>
@@ -12745,9 +12761,8 @@
       <c r="P76" t="str">
         <v/>
       </c>
-      <c r="Q76" t="str" xml:space="preserve">
-        <v xml:space="preserve">Monica is busy with ENGR labs all day Thursday.
-Set as on-hold? we may not have the enrollment.</v>
+      <c r="Q76" t="str">
+        <v/>
       </c>
     </row>
     <row r="77">
@@ -13121,9 +13136,9 @@
         <v/>
       </c>
     </row>
-    <row r="84" xml:space="preserve">
+    <row r="84">
       <c r="A84" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B84" t="str">
         <v>DATA</v>
@@ -13132,7 +13147,7 @@
         <v>102</v>
       </c>
       <c r="D84" t="str">
-        <v>E</v>
+        <v>F</v>
       </c>
       <c r="E84" t="str">
         <v>2</v>
@@ -13141,10 +13156,10 @@
         <v>2</v>
       </c>
       <c r="G84" t="str">
-        <v>MWF</v>
+        <v>TR</v>
       </c>
       <c r="H84" t="str">
-        <v>09:15:00 - 10:20:00</v>
+        <v>12:15:00 - 13:55:00</v>
       </c>
       <c r="I84" t="str">
         <v>SB 354</v>
@@ -13153,16 +13168,16 @@
         <v>Second</v>
       </c>
       <c r="K84" t="str">
-        <v>SP-Second</v>
+        <v>FA-Second</v>
       </c>
       <c r="L84">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="M84" t="str">
         <v>Foundations of Data Science and Analytics</v>
       </c>
       <c r="N84" t="str">
-        <v>Fernando Pasquini Santos</v>
+        <v>Cancelled-DATA</v>
       </c>
       <c r="O84" t="str">
         <v/>
@@ -13170,371 +13185,371 @@
       <c r="P84" t="str">
         <v/>
       </c>
-      <c r="Q84" t="str" xml:space="preserve">
+      <c r="Q84" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>SP</v>
+      </c>
+      <c r="B85" t="str">
+        <v>DATA</v>
+      </c>
+      <c r="C85" t="str">
+        <v>102</v>
+      </c>
+      <c r="D85" t="str">
+        <v>F</v>
+      </c>
+      <c r="E85" t="str">
+        <v>2</v>
+      </c>
+      <c r="F85" t="str">
+        <v>2</v>
+      </c>
+      <c r="G85" t="str">
+        <v>TR</v>
+      </c>
+      <c r="H85" t="str">
+        <v>12:15:00 - 13:55:00</v>
+      </c>
+      <c r="I85" t="str">
+        <v>SB 354</v>
+      </c>
+      <c r="J85" t="str">
+        <v>Second</v>
+      </c>
+      <c r="K85" t="str">
+        <v>SP-Second</v>
+      </c>
+      <c r="L85">
+        <v>100</v>
+      </c>
+      <c r="M85" t="str">
+        <v>Foundations of Data Science and Analytics</v>
+      </c>
+      <c r="N85" t="str">
+        <v>Cancelled-DATA</v>
+      </c>
+      <c r="O85" t="str">
+        <v/>
+      </c>
+      <c r="P85" t="str">
+        <v/>
+      </c>
+      <c r="Q85" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>FA</v>
+      </c>
+      <c r="B86" t="str">
+        <v>DATA</v>
+      </c>
+      <c r="C86" t="str">
+        <v>102</v>
+      </c>
+      <c r="D86" t="str">
+        <v>G</v>
+      </c>
+      <c r="E86" t="str">
+        <v>2</v>
+      </c>
+      <c r="F86" t="str">
+        <v>2</v>
+      </c>
+      <c r="G86" t="str">
+        <v>TR</v>
+      </c>
+      <c r="H86" t="str">
+        <v>14:10:00 - 15:50:00</v>
+      </c>
+      <c r="I86" t="str">
+        <v>SB 354</v>
+      </c>
+      <c r="J86" t="str">
+        <v>Second</v>
+      </c>
+      <c r="K86" t="str">
+        <v>FA-Second</v>
+      </c>
+      <c r="L86">
+        <v>100</v>
+      </c>
+      <c r="M86" t="str">
+        <v>Foundations of Data Science and Analytics</v>
+      </c>
+      <c r="N86" t="str">
+        <v>Cancelled-DATA</v>
+      </c>
+      <c r="O86" t="str">
+        <v/>
+      </c>
+      <c r="P86" t="str">
+        <v/>
+      </c>
+      <c r="Q86" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>SP</v>
+      </c>
+      <c r="B87" t="str">
+        <v>DATA</v>
+      </c>
+      <c r="C87" t="str">
+        <v>102</v>
+      </c>
+      <c r="D87" t="str">
+        <v>G</v>
+      </c>
+      <c r="E87" t="str">
+        <v>2</v>
+      </c>
+      <c r="F87" t="str">
+        <v>2</v>
+      </c>
+      <c r="G87" t="str">
+        <v>TR</v>
+      </c>
+      <c r="H87" t="str">
+        <v>14:10:00 - 15:50:00</v>
+      </c>
+      <c r="I87" t="str">
+        <v>SB 354</v>
+      </c>
+      <c r="J87" t="str">
+        <v>Second</v>
+      </c>
+      <c r="K87" t="str">
+        <v>SP-Second</v>
+      </c>
+      <c r="L87">
+        <v>100</v>
+      </c>
+      <c r="M87" t="str">
+        <v>Foundations of Data Science and Analytics</v>
+      </c>
+      <c r="N87" t="str">
+        <v>Cancelled-DATA</v>
+      </c>
+      <c r="O87" t="str">
+        <v/>
+      </c>
+      <c r="P87" t="str">
+        <v/>
+      </c>
+      <c r="Q87" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>FA</v>
+      </c>
+      <c r="B88" t="str">
+        <v>DATA</v>
+      </c>
+      <c r="C88" t="str">
+        <v>102</v>
+      </c>
+      <c r="D88" t="str">
+        <v>H</v>
+      </c>
+      <c r="E88" t="str">
+        <v>2</v>
+      </c>
+      <c r="F88" t="str">
+        <v>2</v>
+      </c>
+      <c r="G88" t="str">
+        <v>TR</v>
+      </c>
+      <c r="H88" t="str">
+        <v>19:00:00 - 20:40:00</v>
+      </c>
+      <c r="I88" t="str">
+        <v>SB 354</v>
+      </c>
+      <c r="J88" t="str">
+        <v>Second</v>
+      </c>
+      <c r="K88" t="str">
+        <v>FA-Second</v>
+      </c>
+      <c r="L88">
+        <v>100</v>
+      </c>
+      <c r="M88" t="str">
+        <v>Foundations of Data Science and Analytics</v>
+      </c>
+      <c r="N88" t="str">
+        <v>Jim Momeyer</v>
+      </c>
+      <c r="O88" t="str">
+        <v/>
+      </c>
+      <c r="P88" t="str">
+        <v/>
+      </c>
+      <c r="Q88" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>SP</v>
+      </c>
+      <c r="B89" t="str">
+        <v>DATA</v>
+      </c>
+      <c r="C89" t="str">
+        <v>102</v>
+      </c>
+      <c r="D89" t="str">
+        <v>H</v>
+      </c>
+      <c r="E89" t="str">
+        <v>2</v>
+      </c>
+      <c r="F89" t="str">
+        <v>2</v>
+      </c>
+      <c r="G89" t="str">
+        <v>TR</v>
+      </c>
+      <c r="H89" t="str">
+        <v>19:00:00 - 20:40:00</v>
+      </c>
+      <c r="I89" t="str">
+        <v>SB 354</v>
+      </c>
+      <c r="J89" t="str">
+        <v>Second</v>
+      </c>
+      <c r="K89" t="str">
+        <v>SP-Second</v>
+      </c>
+      <c r="L89">
+        <v>100</v>
+      </c>
+      <c r="M89" t="str">
+        <v>Foundations of Data Science and Analytics</v>
+      </c>
+      <c r="N89" t="str">
+        <v>Jim Momeyer</v>
+      </c>
+      <c r="O89" t="str">
+        <v/>
+      </c>
+      <c r="P89" t="str">
+        <v/>
+      </c>
+      <c r="Q89" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="90" xml:space="preserve">
+      <c r="A90" t="str">
+        <v>SP</v>
+      </c>
+      <c r="B90" t="str">
+        <v>DATA</v>
+      </c>
+      <c r="C90" t="str">
+        <v>102</v>
+      </c>
+      <c r="D90" t="str">
+        <v>A</v>
+      </c>
+      <c r="E90" t="str">
+        <v>2</v>
+      </c>
+      <c r="F90" t="str">
+        <v>2</v>
+      </c>
+      <c r="G90" t="str">
+        <v>MWF</v>
+      </c>
+      <c r="H90" t="str">
+        <v>09:15:00 - 10:20:00</v>
+      </c>
+      <c r="I90" t="str">
+        <v>SB 354</v>
+      </c>
+      <c r="J90" t="str">
+        <v>First</v>
+      </c>
+      <c r="K90" t="str">
+        <v>SP-First</v>
+      </c>
+      <c r="L90">
+        <v>65</v>
+      </c>
+      <c r="M90" t="str">
+        <v>Foundations of Data Science and Analytics</v>
+      </c>
+      <c r="N90" t="str">
+        <v>Jim Momeyer</v>
+      </c>
+      <c r="O90" t="str">
+        <v/>
+      </c>
+      <c r="P90" t="str">
+        <v/>
+      </c>
+      <c r="Q90" t="str" xml:space="preserve">
         <v xml:space="preserve">Monica is busy with ENGR labs all day Thursday.
 Set as on-hold? we may not have the enrollment.</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" t="str">
-        <v>FA</v>
-      </c>
-      <c r="B85" t="str">
-        <v>DATA</v>
-      </c>
-      <c r="C85" t="str">
-        <v>102</v>
-      </c>
-      <c r="D85" t="str">
-        <v>F</v>
-      </c>
-      <c r="E85" t="str">
-        <v>2</v>
-      </c>
-      <c r="F85" t="str">
-        <v>2</v>
-      </c>
-      <c r="G85" t="str">
-        <v>TR</v>
-      </c>
-      <c r="H85" t="str">
-        <v>12:15:00 - 13:55:00</v>
-      </c>
-      <c r="I85" t="str">
-        <v>SB 354</v>
-      </c>
-      <c r="J85" t="str">
-        <v>Second</v>
-      </c>
-      <c r="K85" t="str">
-        <v>FA-Second</v>
-      </c>
-      <c r="L85">
-        <v>100</v>
-      </c>
-      <c r="M85" t="str">
-        <v>Foundations of Data Science and Analytics</v>
-      </c>
-      <c r="N85" t="str">
-        <v>Cancelled-DATA</v>
-      </c>
-      <c r="O85" t="str">
-        <v/>
-      </c>
-      <c r="P85" t="str">
-        <v/>
-      </c>
-      <c r="Q85" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="str">
+    <row r="91" xml:space="preserve">
+      <c r="A91" t="str">
         <v>SP</v>
-      </c>
-      <c r="B86" t="str">
-        <v>DATA</v>
-      </c>
-      <c r="C86" t="str">
-        <v>102</v>
-      </c>
-      <c r="D86" t="str">
-        <v>F</v>
-      </c>
-      <c r="E86" t="str">
-        <v>2</v>
-      </c>
-      <c r="F86" t="str">
-        <v>2</v>
-      </c>
-      <c r="G86" t="str">
-        <v>TR</v>
-      </c>
-      <c r="H86" t="str">
-        <v>12:15:00 - 13:55:00</v>
-      </c>
-      <c r="I86" t="str">
-        <v>SB 354</v>
-      </c>
-      <c r="J86" t="str">
-        <v>Second</v>
-      </c>
-      <c r="K86" t="str">
-        <v>SP-Second</v>
-      </c>
-      <c r="L86">
-        <v>100</v>
-      </c>
-      <c r="M86" t="str">
-        <v>Foundations of Data Science and Analytics</v>
-      </c>
-      <c r="N86" t="str">
-        <v>Cancelled-DATA</v>
-      </c>
-      <c r="O86" t="str">
-        <v/>
-      </c>
-      <c r="P86" t="str">
-        <v/>
-      </c>
-      <c r="Q86" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="str">
-        <v>FA</v>
-      </c>
-      <c r="B87" t="str">
-        <v>DATA</v>
-      </c>
-      <c r="C87" t="str">
-        <v>102</v>
-      </c>
-      <c r="D87" t="str">
-        <v>G</v>
-      </c>
-      <c r="E87" t="str">
-        <v>2</v>
-      </c>
-      <c r="F87" t="str">
-        <v>2</v>
-      </c>
-      <c r="G87" t="str">
-        <v>TR</v>
-      </c>
-      <c r="H87" t="str">
-        <v>14:10:00 - 15:50:00</v>
-      </c>
-      <c r="I87" t="str">
-        <v>SB 354</v>
-      </c>
-      <c r="J87" t="str">
-        <v>Second</v>
-      </c>
-      <c r="K87" t="str">
-        <v>FA-Second</v>
-      </c>
-      <c r="L87">
-        <v>100</v>
-      </c>
-      <c r="M87" t="str">
-        <v>Foundations of Data Science and Analytics</v>
-      </c>
-      <c r="N87" t="str">
-        <v>Cancelled-DATA</v>
-      </c>
-      <c r="O87" t="str">
-        <v/>
-      </c>
-      <c r="P87" t="str">
-        <v/>
-      </c>
-      <c r="Q87" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="str">
-        <v>SP</v>
-      </c>
-      <c r="B88" t="str">
-        <v>DATA</v>
-      </c>
-      <c r="C88" t="str">
-        <v>102</v>
-      </c>
-      <c r="D88" t="str">
-        <v>G</v>
-      </c>
-      <c r="E88" t="str">
-        <v>2</v>
-      </c>
-      <c r="F88" t="str">
-        <v>2</v>
-      </c>
-      <c r="G88" t="str">
-        <v>TR</v>
-      </c>
-      <c r="H88" t="str">
-        <v>14:10:00 - 15:50:00</v>
-      </c>
-      <c r="I88" t="str">
-        <v>SB 354</v>
-      </c>
-      <c r="J88" t="str">
-        <v>Second</v>
-      </c>
-      <c r="K88" t="str">
-        <v>SP-Second</v>
-      </c>
-      <c r="L88">
-        <v>100</v>
-      </c>
-      <c r="M88" t="str">
-        <v>Foundations of Data Science and Analytics</v>
-      </c>
-      <c r="N88" t="str">
-        <v>Cancelled-DATA</v>
-      </c>
-      <c r="O88" t="str">
-        <v/>
-      </c>
-      <c r="P88" t="str">
-        <v/>
-      </c>
-      <c r="Q88" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="str">
-        <v>FA</v>
-      </c>
-      <c r="B89" t="str">
-        <v>DATA</v>
-      </c>
-      <c r="C89" t="str">
-        <v>102</v>
-      </c>
-      <c r="D89" t="str">
-        <v>H</v>
-      </c>
-      <c r="E89" t="str">
-        <v>2</v>
-      </c>
-      <c r="F89" t="str">
-        <v>2</v>
-      </c>
-      <c r="G89" t="str">
-        <v>TR</v>
-      </c>
-      <c r="H89" t="str">
-        <v>19:00:00 - 20:40:00</v>
-      </c>
-      <c r="I89" t="str">
-        <v>SB 354</v>
-      </c>
-      <c r="J89" t="str">
-        <v>Second</v>
-      </c>
-      <c r="K89" t="str">
-        <v>FA-Second</v>
-      </c>
-      <c r="L89">
-        <v>100</v>
-      </c>
-      <c r="M89" t="str">
-        <v>Foundations of Data Science and Analytics</v>
-      </c>
-      <c r="N89" t="str">
-        <v>Jim Momeyer</v>
-      </c>
-      <c r="O89" t="str">
-        <v/>
-      </c>
-      <c r="P89" t="str">
-        <v/>
-      </c>
-      <c r="Q89" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="str">
-        <v>SP</v>
-      </c>
-      <c r="B90" t="str">
-        <v>DATA</v>
-      </c>
-      <c r="C90" t="str">
-        <v>102</v>
-      </c>
-      <c r="D90" t="str">
-        <v>H</v>
-      </c>
-      <c r="E90" t="str">
-        <v>2</v>
-      </c>
-      <c r="F90" t="str">
-        <v>2</v>
-      </c>
-      <c r="G90" t="str">
-        <v>TR</v>
-      </c>
-      <c r="H90" t="str">
-        <v>19:00:00 - 20:40:00</v>
-      </c>
-      <c r="I90" t="str">
-        <v>SB 354</v>
-      </c>
-      <c r="J90" t="str">
-        <v>Second</v>
-      </c>
-      <c r="K90" t="str">
-        <v>SP-Second</v>
-      </c>
-      <c r="L90">
-        <v>100</v>
-      </c>
-      <c r="M90" t="str">
-        <v>Foundations of Data Science and Analytics</v>
-      </c>
-      <c r="N90" t="str">
-        <v>Jim Momeyer</v>
-      </c>
-      <c r="O90" t="str">
-        <v/>
-      </c>
-      <c r="P90" t="str">
-        <v/>
-      </c>
-      <c r="Q90" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="str">
-        <v>FA</v>
       </c>
       <c r="B91" t="str">
         <v>DATA</v>
       </c>
       <c r="C91" t="str">
-        <v>202</v>
+        <v>102</v>
       </c>
       <c r="D91" t="str">
-        <v>A</v>
+        <v>E</v>
       </c>
       <c r="E91" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F91" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G91" t="str">
         <v>MWF</v>
       </c>
       <c r="H91" t="str">
-        <v>08:00:00 - 09:05:00</v>
+        <v>09:15:00 - 10:20:00</v>
       </c>
       <c r="I91" t="str">
-        <v>SB 382</v>
+        <v>SB 354</v>
       </c>
       <c r="J91" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="K91" t="str">
-        <v>FA-Full</v>
+        <v>SP-Second</v>
       </c>
       <c r="L91">
         <v>65</v>
       </c>
       <c r="M91" t="str">
-        <v>Predictive Analytics</v>
+        <v>Foundations of Data Science and Analytics</v>
       </c>
       <c r="N91" t="str">
-        <v>Fernando Pasquini Santos</v>
+        <v>Jim Momeyer</v>
       </c>
       <c r="O91" t="str">
         <v/>
@@ -13542,8 +13557,9 @@
       <c r="P91" t="str">
         <v/>
       </c>
-      <c r="Q91" t="str">
-        <v/>
+      <c r="Q91" t="str" xml:space="preserve">
+        <v xml:space="preserve">Monica is busy with ENGR labs all day Thursday.
+Set as on-hold? we may not have the enrollment.</v>
       </c>
     </row>
     <row r="92">
@@ -13557,7 +13573,7 @@
         <v>202</v>
       </c>
       <c r="D92" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="E92" t="str">
         <v>4</v>
@@ -13569,7 +13585,7 @@
         <v>MWF</v>
       </c>
       <c r="H92" t="str">
-        <v>09:15:00 - 10:20:00</v>
+        <v>08:00:00 - 09:05:00</v>
       </c>
       <c r="I92" t="str">
         <v>SB 382</v>
@@ -13607,22 +13623,22 @@
         <v>DATA</v>
       </c>
       <c r="C93" t="str">
-        <v>396</v>
+        <v>202</v>
       </c>
       <c r="D93" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="E93" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F93" t="str">
-        <v>0.3</v>
+        <v>4</v>
       </c>
       <c r="G93" t="str">
-        <v>T</v>
+        <v>MWF</v>
       </c>
       <c r="H93" t="str">
-        <v>19:00:00 - 19:50:00</v>
+        <v>09:15:00 - 10:20:00</v>
       </c>
       <c r="I93" t="str">
         <v>SB 382</v>
@@ -13634,13 +13650,13 @@
         <v>FA-Full</v>
       </c>
       <c r="L93">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="M93" t="str">
-        <v>Senior Project in Data Science</v>
+        <v>Predictive Analytics</v>
       </c>
       <c r="N93" t="str">
-        <v>Kenneth C Arnold</v>
+        <v>Fernando Pasquini Santos</v>
       </c>
       <c r="O93" t="str">
         <v/>
@@ -13654,13 +13670,13 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B94" t="str">
         <v>DATA</v>
       </c>
       <c r="C94" t="str">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D94" t="str">
         <v>A</v>
@@ -13684,13 +13700,13 @@
         <v>Full</v>
       </c>
       <c r="K94" t="str">
-        <v>SP-Full</v>
+        <v>FA-Full</v>
       </c>
       <c r="L94">
         <v>50</v>
       </c>
       <c r="M94" t="str">
-        <v>Senior Project in Data Science II</v>
+        <v>Senior Project in Data Science</v>
       </c>
       <c r="N94" t="str">
         <v>Kenneth C Arnold</v>
@@ -13707,13 +13723,13 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B95" t="str">
         <v>DATA</v>
       </c>
       <c r="C95" t="str">
-        <v>501</v>
+        <v>398</v>
       </c>
       <c r="D95" t="str">
         <v>A</v>
@@ -13722,31 +13738,31 @@
         <v>2</v>
       </c>
       <c r="F95" t="str">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="G95" t="str">
-        <v/>
+        <v>T</v>
       </c>
       <c r="H95" t="str">
-        <v/>
+        <v>19:00:00 - 19:50:00</v>
       </c>
       <c r="I95" t="str">
-        <v/>
+        <v>SB 382</v>
       </c>
       <c r="J95" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="K95" t="str">
-        <v>FA-First</v>
-      </c>
-      <c r="L95" t="str">
-        <v/>
+        <v>SP-Full</v>
+      </c>
+      <c r="L95">
+        <v>50</v>
       </c>
       <c r="M95" t="str">
-        <v>Data Wrangling</v>
+        <v>Senior Project in Data Science II</v>
       </c>
       <c r="N95" t="str">
-        <v>Cancelled-MDS</v>
+        <v>Kenneth C Arnold</v>
       </c>
       <c r="O95" t="str">
         <v/>
@@ -13766,7 +13782,7 @@
         <v>DATA</v>
       </c>
       <c r="C96" t="str">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D96" t="str">
         <v>A</v>
@@ -13787,16 +13803,16 @@
         <v/>
       </c>
       <c r="J96" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="K96" t="str">
-        <v>FA-Second</v>
+        <v>FA-First</v>
       </c>
       <c r="L96" t="str">
         <v/>
       </c>
       <c r="M96" t="str">
-        <v>Introduction to Machine Learning</v>
+        <v>Data Wrangling</v>
       </c>
       <c r="N96" t="str">
         <v>Cancelled-MDS</v>
@@ -13813,13 +13829,13 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>SU</v>
+        <v>FA</v>
       </c>
       <c r="B97" t="str">
         <v>DATA</v>
       </c>
       <c r="C97" t="str">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D97" t="str">
         <v>A</v>
@@ -13840,16 +13856,16 @@
         <v/>
       </c>
       <c r="J97" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="K97" t="str">
-        <v>SU-First</v>
+        <v>FA-Second</v>
       </c>
       <c r="L97" t="str">
         <v/>
       </c>
       <c r="M97" t="str">
-        <v>Visualization for Data Science</v>
+        <v>Introduction to Machine Learning</v>
       </c>
       <c r="N97" t="str">
         <v>Cancelled-MDS</v>
@@ -13866,13 +13882,13 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>SP</v>
+        <v>SU</v>
       </c>
       <c r="B98" t="str">
         <v>DATA</v>
       </c>
       <c r="C98" t="str">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="D98" t="str">
         <v>A</v>
@@ -13896,13 +13912,13 @@
         <v>First</v>
       </c>
       <c r="K98" t="str">
-        <v>SP-First</v>
+        <v>SU-First</v>
       </c>
       <c r="L98" t="str">
         <v/>
       </c>
       <c r="M98" t="str">
-        <v>Ethics for Data Science</v>
+        <v>Visualization for Data Science</v>
       </c>
       <c r="N98" t="str">
         <v>Cancelled-MDS</v>
@@ -13919,13 +13935,13 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>SU</v>
+        <v>SP</v>
       </c>
       <c r="B99" t="str">
         <v>DATA</v>
       </c>
       <c r="C99" t="str">
-        <v>539</v>
+        <v>510</v>
       </c>
       <c r="D99" t="str">
         <v>A</v>
@@ -13946,16 +13962,16 @@
         <v/>
       </c>
       <c r="J99" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="K99" t="str">
-        <v>SU-Second</v>
+        <v>SP-First</v>
       </c>
       <c r="L99" t="str">
         <v/>
       </c>
       <c r="M99" t="str">
-        <v>Administering Cloud Services</v>
+        <v>Ethics for Data Science</v>
       </c>
       <c r="N99" t="str">
         <v>Cancelled-MDS</v>
@@ -13972,22 +13988,22 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>SP</v>
+        <v>SU</v>
       </c>
       <c r="B100" t="str">
         <v>DATA</v>
       </c>
       <c r="C100" t="str">
-        <v>562</v>
+        <v>539</v>
       </c>
       <c r="D100" t="str">
         <v>A</v>
       </c>
       <c r="E100" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F100" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G100" t="str">
         <v/>
@@ -13999,16 +14015,16 @@
         <v/>
       </c>
       <c r="J100" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="K100" t="str">
-        <v>SP-Full</v>
+        <v>SU-Second</v>
       </c>
       <c r="L100" t="str">
         <v/>
       </c>
       <c r="M100" t="str">
-        <v>Systems Engineering for Data Science</v>
+        <v>Administering Cloud Services</v>
       </c>
       <c r="N100" t="str">
         <v>Cancelled-MDS</v>
@@ -14025,22 +14041,22 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>SU</v>
+        <v>SP</v>
       </c>
       <c r="B101" t="str">
         <v>DATA</v>
       </c>
       <c r="C101" t="str">
-        <v>654</v>
+        <v>562</v>
       </c>
       <c r="D101" t="str">
         <v>A</v>
       </c>
       <c r="E101" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F101" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G101" t="str">
         <v/>
@@ -14052,16 +14068,16 @@
         <v/>
       </c>
       <c r="J101" t="str">
-        <v>Second</v>
+        <v>Full</v>
       </c>
       <c r="K101" t="str">
-        <v>SU-Second</v>
+        <v>SP-Full</v>
       </c>
       <c r="L101" t="str">
         <v/>
       </c>
       <c r="M101" t="str">
-        <v>Database Management Systems</v>
+        <v>Systems Engineering for Data Science</v>
       </c>
       <c r="N101" t="str">
         <v>Cancelled-MDS</v>
@@ -14078,13 +14094,13 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>SP</v>
+        <v>SU</v>
       </c>
       <c r="B102" t="str">
         <v>DATA</v>
       </c>
       <c r="C102" t="str">
-        <v>675</v>
+        <v>654</v>
       </c>
       <c r="D102" t="str">
         <v>A</v>
@@ -14108,13 +14124,13 @@
         <v>Second</v>
       </c>
       <c r="K102" t="str">
-        <v>SP-Second</v>
+        <v>SU-Second</v>
       </c>
       <c r="L102" t="str">
         <v/>
       </c>
       <c r="M102" t="str">
-        <v>Introduction to Deep Learning</v>
+        <v>Database Management Systems</v>
       </c>
       <c r="N102" t="str">
         <v>Cancelled-MDS</v>
@@ -14131,13 +14147,13 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>SU</v>
+        <v>SP</v>
       </c>
       <c r="B103" t="str">
         <v>DATA</v>
       </c>
       <c r="C103" t="str">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D103" t="str">
         <v>A</v>
@@ -14158,16 +14174,16 @@
         <v/>
       </c>
       <c r="J103" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="K103" t="str">
-        <v>SU-First</v>
+        <v>SP-Second</v>
       </c>
       <c r="L103" t="str">
         <v/>
       </c>
       <c r="M103" t="str">
-        <v>Deep Learning for Text and Generative Models</v>
+        <v>Introduction to Deep Learning</v>
       </c>
       <c r="N103" t="str">
         <v>Cancelled-MDS</v>
@@ -14190,7 +14206,7 @@
         <v>DATA</v>
       </c>
       <c r="C104" t="str">
-        <v>696</v>
+        <v>676</v>
       </c>
       <c r="D104" t="str">
         <v>A</v>
@@ -14211,16 +14227,16 @@
         <v/>
       </c>
       <c r="J104" t="str">
-        <v>Full</v>
+        <v>First</v>
       </c>
       <c r="K104" t="str">
-        <v>SU-Full</v>
+        <v>SU-First</v>
       </c>
       <c r="L104" t="str">
         <v/>
       </c>
       <c r="M104" t="str">
-        <v>Project in Data Science</v>
+        <v>Deep Learning for Text and Generative Models</v>
       </c>
       <c r="N104" t="str">
         <v>Cancelled-MDS</v>
@@ -14243,7 +14259,7 @@
         <v>DATA</v>
       </c>
       <c r="C105" t="str">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="D105" t="str">
         <v>A</v>
@@ -14264,10 +14280,10 @@
         <v/>
       </c>
       <c r="J105" t="str">
-        <v>Second</v>
+        <v>Full</v>
       </c>
       <c r="K105" t="str">
-        <v>SU-Second</v>
+        <v>SU-Full</v>
       </c>
       <c r="L105" t="str">
         <v/>
@@ -14290,13 +14306,13 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>FA</v>
+        <v>SU</v>
       </c>
       <c r="B106" t="str">
-        <v>HNRS</v>
+        <v>DATA</v>
       </c>
       <c r="C106" t="str">
-        <v>251</v>
+        <v>698</v>
       </c>
       <c r="D106" t="str">
         <v>A</v>
@@ -14308,28 +14324,28 @@
         <v>2</v>
       </c>
       <c r="G106" t="str">
-        <v>TR</v>
+        <v/>
       </c>
       <c r="H106" t="str">
-        <v>14:10:00 - 15:15:00</v>
+        <v/>
       </c>
       <c r="I106" t="str">
-        <v>HL 406C</v>
+        <v/>
       </c>
       <c r="J106" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="K106" t="str">
-        <v>FA-Full</v>
-      </c>
-      <c r="L106">
-        <v>65</v>
+        <v>SU-Second</v>
+      </c>
+      <c r="L106" t="str">
+        <v/>
       </c>
       <c r="M106" t="str">
-        <v>Agent Modeling</v>
+        <v>Project in Data Science</v>
       </c>
       <c r="N106" t="str">
-        <v>Eric Araujo</v>
+        <v>Cancelled-MDS</v>
       </c>
       <c r="O106" t="str">
         <v/>
@@ -14346,43 +14362,43 @@
         <v>FA</v>
       </c>
       <c r="B107" t="str">
-        <v>CS</v>
+        <v>HNRS</v>
       </c>
       <c r="C107" t="str">
-        <v>300-S</v>
+        <v>251</v>
       </c>
       <c r="D107" t="str">
-        <v>A-S</v>
+        <v>A</v>
       </c>
       <c r="E107" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F107" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G107" t="str">
-        <v>MWF</v>
+        <v>TR</v>
       </c>
       <c r="H107" t="str">
-        <v>11:00:00 - 12:05:00</v>
+        <v>14:10:00 - 15:15:00</v>
       </c>
       <c r="I107" t="str">
-        <v>SB 354</v>
+        <v>HL 406C</v>
       </c>
       <c r="J107" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="K107" t="str">
-        <v>FA-First</v>
+        <v>FA-Full</v>
       </c>
       <c r="L107">
         <v>65</v>
       </c>
       <c r="M107" t="str">
-        <v>Applied Machine Learning</v>
+        <v>Agent Modeling</v>
       </c>
       <c r="N107" t="str">
-        <v>Shadow-Gold</v>
+        <v>Eric Araujo</v>
       </c>
       <c r="O107" t="str">
         <v/>
@@ -14396,7 +14412,7 @@
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B108" t="str">
         <v>CS</v>
@@ -14417,16 +14433,16 @@
         <v>MWF</v>
       </c>
       <c r="H108" t="str">
-        <v>12:15:00 - 13:20:00</v>
+        <v>11:00:00 - 12:05:00</v>
       </c>
       <c r="I108" t="str">
         <v>SB 354</v>
       </c>
       <c r="J108" t="str">
-        <v>Full</v>
+        <v>First</v>
       </c>
       <c r="K108" t="str">
-        <v>SP-Full</v>
+        <v>FA-First</v>
       </c>
       <c r="L108">
         <v>65</v>
@@ -14449,7 +14465,7 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B109" t="str">
         <v>CS</v>
@@ -14458,7 +14474,7 @@
         <v>300-S</v>
       </c>
       <c r="D109" t="str">
-        <v>B-S</v>
+        <v>A-S</v>
       </c>
       <c r="E109" t="str">
         <v>0</v>
@@ -14470,16 +14486,16 @@
         <v>MWF</v>
       </c>
       <c r="H109" t="str">
-        <v>11:00:00 - 12:05:00</v>
+        <v>12:15:00 - 13:20:00</v>
       </c>
       <c r="I109" t="str">
         <v>SB 354</v>
       </c>
       <c r="J109" t="str">
-        <v>Second</v>
+        <v>Full</v>
       </c>
       <c r="K109" t="str">
-        <v>FA-Second</v>
+        <v>SP-Full</v>
       </c>
       <c r="L109">
         <v>65</v>
@@ -14502,16 +14518,16 @@
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B110" t="str">
         <v>CS</v>
       </c>
       <c r="C110" t="str">
-        <v>338-S</v>
+        <v>300-S</v>
       </c>
       <c r="D110" t="str">
-        <v>A-S</v>
+        <v>B-S</v>
       </c>
       <c r="E110" t="str">
         <v>0</v>
@@ -14523,22 +14539,22 @@
         <v>MWF</v>
       </c>
       <c r="H110" t="str">
-        <v>08:00:00 - 09:05:00</v>
+        <v>11:00:00 - 12:05:00</v>
       </c>
       <c r="I110" t="str">
         <v>SB 354</v>
       </c>
       <c r="J110" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="K110" t="str">
-        <v>SP-First</v>
+        <v>FA-Second</v>
       </c>
       <c r="L110">
         <v>65</v>
       </c>
       <c r="M110" t="str">
-        <v>System Administration: Infrastructure</v>
+        <v>Applied Machine Learning</v>
       </c>
       <c r="N110" t="str">
         <v>Shadow-Gold</v>
@@ -14561,7 +14577,7 @@
         <v>CS</v>
       </c>
       <c r="C111" t="str">
-        <v>339-S</v>
+        <v>338-S</v>
       </c>
       <c r="D111" t="str">
         <v>A-S</v>
@@ -14582,16 +14598,16 @@
         <v>SB 354</v>
       </c>
       <c r="J111" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="K111" t="str">
-        <v>SP-Second</v>
+        <v>SP-First</v>
       </c>
       <c r="L111">
         <v>65</v>
       </c>
       <c r="M111" t="str">
-        <v>System Administration: Cloud Services</v>
+        <v>System Administration: Infrastructure</v>
       </c>
       <c r="N111" t="str">
         <v>Shadow-Gold</v>
@@ -14608,28 +14624,28 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B112" t="str">
         <v>CS</v>
       </c>
       <c r="C112" t="str">
-        <v>374-S</v>
+        <v>339-S</v>
       </c>
       <c r="D112" t="str">
         <v>A-S</v>
       </c>
       <c r="E112" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F112" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G112" t="str">
-        <v>MW</v>
+        <v>MWF</v>
       </c>
       <c r="H112" t="str">
-        <v>14:45:00 - 15:50:00</v>
+        <v>08:00:00 - 09:05:00</v>
       </c>
       <c r="I112" t="str">
         <v>SB 354</v>
@@ -14638,13 +14654,13 @@
         <v>Second</v>
       </c>
       <c r="K112" t="str">
-        <v>FA-Second</v>
+        <v>SP-Second</v>
       </c>
       <c r="L112">
         <v>65</v>
       </c>
       <c r="M112" t="str">
-        <v>High-Performance Computing</v>
+        <v>System Administration: Cloud Services</v>
       </c>
       <c r="N112" t="str">
         <v>Shadow-Gold</v>
@@ -14661,43 +14677,43 @@
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B113" t="str">
         <v>CS</v>
       </c>
       <c r="C113" t="str">
-        <v>375-S</v>
+        <v>374-S</v>
       </c>
       <c r="D113" t="str">
         <v>A-S</v>
       </c>
       <c r="E113" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F113" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G113" t="str">
-        <v>MWF</v>
+        <v>MW</v>
       </c>
       <c r="H113" t="str">
-        <v>11:00:00 - 12:05:00</v>
+        <v>14:45:00 - 15:50:00</v>
       </c>
       <c r="I113" t="str">
         <v>SB 354</v>
       </c>
       <c r="J113" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="K113" t="str">
-        <v>SP-First</v>
+        <v>FA-Second</v>
       </c>
       <c r="L113">
         <v>65</v>
       </c>
       <c r="M113" t="str">
-        <v>Artificial Intelligence</v>
+        <v>High-Performance Computing</v>
       </c>
       <c r="N113" t="str">
         <v>Shadow-Gold</v>
@@ -14720,10 +14736,10 @@
         <v>CS</v>
       </c>
       <c r="C114" t="str">
-        <v>376-S</v>
+        <v>375-S</v>
       </c>
       <c r="D114" t="str">
-        <v>B-S</v>
+        <v>A-S</v>
       </c>
       <c r="E114" t="str">
         <v>0</v>
@@ -14741,16 +14757,16 @@
         <v>SB 354</v>
       </c>
       <c r="J114" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="K114" t="str">
-        <v>SP-Second</v>
+        <v>SP-First</v>
       </c>
       <c r="L114">
         <v>65</v>
       </c>
       <c r="M114" t="str">
-        <v>Machine Learning</v>
+        <v>Artificial Intelligence</v>
       </c>
       <c r="N114" t="str">
         <v>Shadow-Gold</v>
@@ -14767,16 +14783,16 @@
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B115" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="C115" t="str">
-        <v>202-S</v>
+        <v>376-S</v>
       </c>
       <c r="D115" t="str">
-        <v>A-S</v>
+        <v>B-S</v>
       </c>
       <c r="E115" t="str">
         <v>0</v>
@@ -14788,25 +14804,25 @@
         <v>MWF</v>
       </c>
       <c r="H115" t="str">
-        <v>08:00:00 - 09:05:00</v>
+        <v>11:00:00 - 12:05:00</v>
       </c>
       <c r="I115" t="str">
         <v>SB 354</v>
       </c>
       <c r="J115" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="K115" t="str">
-        <v>FA-Full</v>
+        <v>SP-Second</v>
       </c>
       <c r="L115">
         <v>65</v>
       </c>
       <c r="M115" t="str">
-        <v>Predictive Analytics</v>
+        <v>Machine Learning</v>
       </c>
       <c r="N115" t="str">
-        <v>Shadow-Maroon</v>
+        <v>Shadow-Gold</v>
       </c>
       <c r="O115" t="str">
         <v/>
@@ -14829,7 +14845,7 @@
         <v>202-S</v>
       </c>
       <c r="D116" t="str">
-        <v>B-S</v>
+        <v>A-S</v>
       </c>
       <c r="E116" t="str">
         <v>0</v>
@@ -14841,7 +14857,7 @@
         <v>MWF</v>
       </c>
       <c r="H116" t="str">
-        <v>09:15:00 - 10:20:00</v>
+        <v>08:00:00 - 09:05:00</v>
       </c>
       <c r="I116" t="str">
         <v>SB 354</v>
@@ -14876,28 +14892,28 @@
         <v>FA</v>
       </c>
       <c r="B117" t="str">
-        <v>CS</v>
+        <v>DATA</v>
       </c>
       <c r="C117" t="str">
-        <v>364</v>
+        <v>202-S</v>
       </c>
       <c r="D117" t="str">
-        <v>A</v>
+        <v>B-S</v>
       </c>
       <c r="E117" t="str">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F117" t="str">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G117" t="str">
-        <v>MR</v>
+        <v>MWF</v>
       </c>
       <c r="H117" t="str">
-        <v>19:00:00 - 20:40:00</v>
+        <v>09:15:00 - 10:20:00</v>
       </c>
       <c r="I117" t="str">
-        <v>SB 372</v>
+        <v>SB 354</v>
       </c>
       <c r="J117" t="str">
         <v>Full</v>
@@ -14906,13 +14922,13 @@
         <v>FA-Full</v>
       </c>
       <c r="L117">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="M117" t="str">
-        <v>Computer Security</v>
+        <v>Predictive Analytics</v>
       </c>
       <c r="N117" t="str">
-        <v>Brian D Paige</v>
+        <v>Shadow-Maroon</v>
       </c>
       <c r="O117" t="str">
         <v/>
@@ -14945,7 +14961,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-09-27 11:30:49</v>
+        <v>2025-11-11 14:06:52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>